<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-21 12:30:04
</commit_message>
<xml_diff>
--- a/BacklogGATEAutoCompleto.xlsx
+++ b/BacklogGATEAutoCompleto.xlsx
@@ -13429,7 +13429,7 @@
     </row>
     <row r="139" spans="1:12">
       <c r="A139" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B139" t="s">
         <v>181</v>
@@ -13450,7 +13450,7 @@
         <v>1685</v>
       </c>
       <c r="I139" t="s">
-        <v>1784</v>
+        <v>1730</v>
       </c>
       <c r="J139" t="s">
         <v>1985</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-02 12:30:03
</commit_message>
<xml_diff>
--- a/BacklogGATEAutoCompleto.xlsx
+++ b/BacklogGATEAutoCompleto.xlsx
@@ -18893,7 +18893,7 @@
     </row>
     <row r="315" spans="1:12">
       <c r="A315" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B315" t="s">
         <v>354</v>
@@ -18914,7 +18914,7 @@
         <v>1533</v>
       </c>
       <c r="I315" t="s">
-        <v>1616</v>
+        <v>1574</v>
       </c>
       <c r="J315" t="s">
         <v>1976</v>
@@ -19068,7 +19068,7 @@
     </row>
     <row r="320" spans="1:12">
       <c r="A320" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B320" t="s">
         <v>359</v>
@@ -19089,7 +19089,7 @@
         <v>1533</v>
       </c>
       <c r="I320" t="s">
-        <v>1616</v>
+        <v>1574</v>
       </c>
       <c r="J320" t="s">
         <v>1981</v>

</xml_diff>